<commit_message>
Initial Testing on the craft
</commit_message>
<xml_diff>
--- a/Report/Report Sections/Glossary.xlsx
+++ b/Report/Report Sections/Glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Waller\Documents\GitHub\Final-Year-Project\Report\Report Sections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Git/Final_Year_Project/Report/Report Sections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB61F784-8201-4C43-9146-72AE850781A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DB0B17-DA0E-7A45-A841-5DC6DBE97E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-6675" yWindow="4755" windowWidth="13500" windowHeight="20835" xr2:uid="{4DA3436A-B789-47A2-9559-5F6B6E3CFF4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13500" windowHeight="15800" xr2:uid="{4DA3436A-B789-47A2-9559-5F6B6E3CFF4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>O.R.C.A - On-water Rubbish Collection robot with Automated sensing</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>SMT - Surface Mount Technology</t>
+  </si>
+  <si>
+    <t>RTOS - Real Time Operating System</t>
+  </si>
+  <si>
+    <t>BLDCM - Brushless DC Motor</t>
+  </si>
+  <si>
+    <t>DC - Direct Current</t>
   </si>
 </sst>
 </file>
@@ -401,40 +410,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBB5749-5208-4CD5-91B3-0C10CF2AC3B6}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>